<commit_message>
cosmetic chagnes and fix 10 team bracket
</commit_message>
<xml_diff>
--- a/agave/BuildBracketFromLL.xlsx
+++ b/agave/BuildBracketFromLL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27630"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\bbld\agave\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\active\bbld\agave\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E3074A0-F08C-4FAB-AE83-92FEC70B5080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0CA2CB-6518-4061-A35F-A18AB92BBCAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{29734B7B-1933-4571-98DE-8ACA796B5F7A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{29734B7B-1933-4571-98DE-8ACA796B5F7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
   <si>
     <t>Top</t>
   </si>
@@ -86,9 +86,6 @@
     <t>T6</t>
   </si>
   <si>
-    <t>B7</t>
-  </si>
-  <si>
     <t>TopKey</t>
   </si>
   <si>
@@ -125,27 +122,15 @@
     <t>J</t>
   </si>
   <si>
-    <t>K</t>
-  </si>
-  <si>
     <t>T5</t>
   </si>
   <si>
     <t>B6</t>
   </si>
   <si>
-    <t>T7</t>
-  </si>
-  <si>
     <t>T13</t>
   </si>
   <si>
-    <t>B13</t>
-  </si>
-  <si>
-    <t>T14</t>
-  </si>
-  <si>
     <t>B14</t>
   </si>
   <si>
@@ -164,9 +149,6 @@
     <t>T15</t>
   </si>
   <si>
-    <t>T17</t>
-  </si>
-  <si>
     <t>B17</t>
   </si>
   <si>
@@ -179,15 +161,6 @@
     <t>T20</t>
   </si>
   <si>
-    <t>B19</t>
-  </si>
-  <si>
-    <t>B20</t>
-  </si>
-  <si>
-    <t>T21</t>
-  </si>
-  <si>
     <t>LosertTo2</t>
   </si>
   <si>
@@ -221,10 +194,22 @@
     <t>Team 10</t>
   </si>
   <si>
-    <t>Team 11</t>
-  </si>
-  <si>
-    <t>T22</t>
+    <t>T12</t>
+  </si>
+  <si>
+    <t>T9</t>
+  </si>
+  <si>
+    <t>B10</t>
+  </si>
+  <si>
+    <t>B15</t>
+  </si>
+  <si>
+    <t>T16</t>
+  </si>
+  <si>
+    <t>T19</t>
   </si>
 </sst>
 </file>
@@ -299,18 +284,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{542EA4E5-B7DE-4EDF-813D-C3DE4748C45C}" name="Table1" displayName="Table1" ref="C4:K52" totalsRowShown="0">
-  <autoFilter ref="C4:K52" xr:uid="{542EA4E5-B7DE-4EDF-813D-C3DE4748C45C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{542EA4E5-B7DE-4EDF-813D-C3DE4748C45C}" name="Table1" displayName="Table1" ref="C4:K51" totalsRowShown="0">
+  <autoFilter ref="C4:K51" xr:uid="{542EA4E5-B7DE-4EDF-813D-C3DE4748C45C}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{4C0C5E91-6B0B-457C-BF5A-8C2123C33FD7}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{6AA8BDCD-D53E-4506-BE05-B3345E7C3F8E}" name="Top" dataDxfId="1">
+    <tableColumn id="2" xr3:uid="{6AA8BDCD-D53E-4506-BE05-B3345E7C3F8E}" name="Top" dataDxfId="3">
       <calculatedColumnFormula>IFERROR(
 IF(Table1[[#This Row],[TopKey]]&lt;&gt;"",
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[TopKey]],Table1[LoserTo],0))),
 IF(LEN( INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&lt;4,"W" &amp;  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EF3517F7-DD79-4584-A543-28CCCE216912}" name="Bottom" dataDxfId="0">
+    <tableColumn id="3" xr3:uid="{EF3517F7-DD79-4584-A543-28CCCE216912}" name="Bottom" dataDxfId="2">
       <calculatedColumnFormula>IFERROR(
 IF(Table1[[#This Row],[BottomKey]]&lt;&gt;"",
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[BottomKey]],Table1[LoserTo],0))),
@@ -321,14 +306,14 @@
     <tableColumn id="6" xr3:uid="{8C2E9631-C8E0-44D4-9D42-D69AC27E056B}" name="BottomKey"/>
     <tableColumn id="4" xr3:uid="{B95FEAA5-1D4C-471C-A8DE-E35389E9ED63}" name="LoserTo"/>
     <tableColumn id="5" xr3:uid="{37CAB2FF-5E03-48B1-A330-777D8A7D280B}" name="WinnerTo"/>
-    <tableColumn id="9" xr3:uid="{2395D99A-2056-4AC7-96EA-B5A0A551BFDF}" name="LosertTo2" dataDxfId="2">
+    <tableColumn id="9" xr3:uid="{2395D99A-2056-4AC7-96EA-B5A0A551BFDF}" name="LosertTo2" dataDxfId="1">
       <calculatedColumnFormula>IFERROR(
 IF(
 ISERROR(MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0)),
     "B" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[BottomKey],0)),
     "T" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{DA795720-B4C2-4FF8-BEC6-68EB57930E4A}" name="Column2" dataDxfId="3">
+    <tableColumn id="8" xr3:uid="{DA795720-B4C2-4FF8-BEC6-68EB57930E4A}" name="Column2" dataDxfId="0">
       <calculatedColumnFormula>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -653,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E8693DC-8547-4432-B039-DC1A3BAC5ED7}">
-  <dimension ref="C4:K52"/>
+  <dimension ref="C4:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="K15" sqref="K15:K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -681,10 +666,10 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
         <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>18</v>
       </c>
       <c r="H4" t="s">
         <v>2</v>
@@ -693,7 +678,7 @@
         <v>3</v>
       </c>
       <c r="J4" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="K4" t="s">
         <v>5</v>
@@ -701,7 +686,7 @@
     </row>
     <row r="5" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D5" t="str">
         <f>IFERROR(
@@ -737,7 +722,7 @@
     </row>
     <row r="6" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D6" t="str">
         <f>IFERROR(
@@ -773,7 +758,7 @@
     </row>
     <row r="7" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D7" t="str">
         <f>IFERROR(
@@ -809,7 +794,7 @@
     </row>
     <row r="8" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D8" t="str">
         <f>IFERROR(
@@ -845,7 +830,7 @@
     </row>
     <row r="9" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D9" t="str">
         <f>IFERROR(
@@ -881,7 +866,7 @@
     </row>
     <row r="10" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D10" t="str">
         <f>IFERROR(
@@ -917,7 +902,7 @@
     </row>
     <row r="11" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D11" t="str">
         <f>IFERROR(
@@ -936,7 +921,7 @@
         <v/>
       </c>
       <c r="I11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J11" t="str">
         <f>IFERROR(
@@ -948,12 +933,12 @@
       </c>
       <c r="K11" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "T4", loser: "", topSource: "", bottomSource: "" },</v>
+        <v>{ winner: "B5", loser: "", topSource: "", bottomSource: "" },</v>
       </c>
     </row>
     <row r="12" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D12" t="str">
         <f>IFERROR(
@@ -972,7 +957,7 @@
         <v/>
       </c>
       <c r="I12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J12" t="str">
         <f>IFERROR(
@@ -984,12 +969,12 @@
       </c>
       <c r="K12" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "B4", loser: "", topSource: "", bottomSource: "" },</v>
+        <v>{ winner: "T6", loser: "", topSource: "", bottomSource: "" },</v>
       </c>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D13" t="str">
         <f>IFERROR(
@@ -1008,7 +993,7 @@
         <v/>
       </c>
       <c r="I13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J13" t="str">
         <f>IFERROR(
@@ -1020,12 +1005,12 @@
       </c>
       <c r="K13" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "B5", loser: "", topSource: "", bottomSource: "" },</v>
+        <v>{ winner: "T4", loser: "", topSource: "", bottomSource: "" },</v>
       </c>
     </row>
     <row r="14" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D14" t="str">
         <f>IFERROR(
@@ -1044,7 +1029,7 @@
         <v/>
       </c>
       <c r="I14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J14" t="str">
         <f>IFERROR(
@@ -1056,12 +1041,12 @@
       </c>
       <c r="K14" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "T6", loser: "", topSource: "", bottomSource: "" },</v>
+        <v>{ winner: "B4", loser: "", topSource: "", bottomSource: "" },</v>
       </c>
     </row>
     <row r="15" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C15" t="s">
-        <v>61</v>
+      <c r="C15">
+        <v>1</v>
       </c>
       <c r="D15" t="str">
         <f>IFERROR(
@@ -1069,7 +1054,7 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[TopKey]],Table1[LoserTo],0))),
 IF(LEN( INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&lt;4,"W" &amp;  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v/>
+        <v>Team 1</v>
       </c>
       <c r="E15" t="str">
         <f>IFERROR(
@@ -1077,10 +1062,13 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[BottomKey]],Table1[LoserTo],0))),
 IF(LEN(INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&gt;4,INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),"W" &amp; INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v/>
+        <v>Team 2</v>
+      </c>
+      <c r="H15" t="s">
+        <v>22</v>
       </c>
       <c r="I15" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="J15" t="str">
         <f>IFERROR(
@@ -1088,16 +1076,16 @@
 ISERROR(MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0)),
     "B" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[BottomKey],0)),
     "T" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0))),"")</f>
-        <v/>
+        <v>T8</v>
       </c>
       <c r="K15" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "B7", loser: "", topSource: "", bottomSource: "" },</v>
+        <v>{ winner: "T5", loser: "T8", topSource: "Team 1", bottomSource: "Team 2" },</v>
       </c>
     </row>
     <row r="16" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" t="str">
         <f>IFERROR(
@@ -1105,7 +1093,7 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[TopKey]],Table1[LoserTo],0))),
 IF(LEN( INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&lt;4,"W" &amp;  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>Team 1</v>
+        <v>Team 3</v>
       </c>
       <c r="E16" t="str">
         <f>IFERROR(
@@ -1113,13 +1101,13 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[BottomKey]],Table1[LoserTo],0))),
 IF(LEN(INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&gt;4,INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),"W" &amp; INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>Team 2</v>
+        <v>Team 4</v>
       </c>
       <c r="H16" t="s">
         <v>19</v>
       </c>
       <c r="I16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J16" t="str">
         <f>IFERROR(
@@ -1127,16 +1115,16 @@
 ISERROR(MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0)),
     "B" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[BottomKey],0)),
     "T" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0))),"")</f>
-        <v>T10</v>
+        <v>B7</v>
       </c>
       <c r="K16" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "T5", loser: "T10", topSource: "Team 1", bottomSource: "Team 2" },</v>
+        <v>{ winner: "B6", loser: "B7", topSource: "Team 3", bottomSource: "Team 4" },</v>
       </c>
     </row>
     <row r="17" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D17" t="str">
         <f>IFERROR(
@@ -1144,7 +1132,7 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[TopKey]],Table1[LoserTo],0))),
 IF(LEN( INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&lt;4,"W" &amp;  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>Team 3</v>
+        <v>Team 5</v>
       </c>
       <c r="E17" t="str">
         <f>IFERROR(
@@ -1152,13 +1140,13 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[BottomKey]],Table1[LoserTo],0))),
 IF(LEN(INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&gt;4,INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),"W" &amp; INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>Team 4</v>
+        <v>Team 6</v>
       </c>
       <c r="H17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J17" t="str">
         <f>IFERROR(
@@ -1166,16 +1154,16 @@
 ISERROR(MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0)),
     "B" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[BottomKey],0)),
     "T" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0))),"")</f>
-        <v>B8</v>
+        <v>T7</v>
       </c>
       <c r="K17" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "B6", loser: "B8", topSource: "Team 3", bottomSource: "Team 4" },</v>
+        <v>{ winner: "T11", loser: "T7", topSource: "Team 5", bottomSource: "Team 6" },</v>
       </c>
     </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D18" t="str">
         <f>IFERROR(
@@ -1183,7 +1171,7 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[TopKey]],Table1[LoserTo],0))),
 IF(LEN( INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&lt;4,"W" &amp;  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>Team 5</v>
+        <v>Team 9</v>
       </c>
       <c r="E18" t="str">
         <f>IFERROR(
@@ -1191,13 +1179,13 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[BottomKey]],Table1[LoserTo],0))),
 IF(LEN(INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&gt;4,INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),"W" &amp; INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>Team 6</v>
+        <v>Team 10</v>
       </c>
       <c r="H18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J18" t="str">
         <f>IFERROR(
@@ -1205,16 +1193,16 @@
 ISERROR(MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0)),
     "B" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[BottomKey],0)),
     "T" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0))),"")</f>
-        <v>B9</v>
+        <v>B8</v>
       </c>
       <c r="K18" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "T7", loser: "B9", topSource: "Team 5", bottomSource: "Team 6" },</v>
+        <v>{ winner: "B12", loser: "B8", topSource: "Team 9", bottomSource: "Team 10" },</v>
       </c>
     </row>
     <row r="19" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D19" t="str">
         <f>IFERROR(
@@ -1222,18 +1210,18 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[TopKey]],Table1[LoserTo],0))),
 IF(LEN( INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&lt;4,"W" &amp;  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
+        <v>W1</v>
+      </c>
+      <c r="E19" t="str">
+        <f>IFERROR(
+IF(Table1[[#This Row],[BottomKey]]&lt;&gt;"",
+_xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[BottomKey]],Table1[LoserTo],0))),
+IF(LEN(INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&gt;4,INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),"W" &amp; INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
+),"")</f>
         <v>Team 7</v>
       </c>
-      <c r="E19" t="str">
-        <f>IFERROR(
-IF(Table1[[#This Row],[BottomKey]]&lt;&gt;"",
-_xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[BottomKey]],Table1[LoserTo],0))),
-IF(LEN(INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&gt;4,INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),"W" &amp; INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
-),"")</f>
-        <v>Team 8</v>
-      </c>
       <c r="H19" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I19" t="s">
         <v>33</v>
@@ -1244,16 +1232,16 @@
 ISERROR(MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0)),
     "B" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[BottomKey],0)),
     "T" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0))),"")</f>
-        <v>T8</v>
+        <v>B9</v>
       </c>
       <c r="K19" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "T13", loser: "T8", topSource: "Team 7", bottomSource: "Team 8" },</v>
+        <v>{ winner: "B11", loser: "B9", topSource: "W1", bottomSource: "Team 7" },</v>
       </c>
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C20">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D20" t="str">
         <f>IFERROR(
@@ -1261,7 +1249,7 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[TopKey]],Table1[LoserTo],0))),
 IF(LEN( INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&lt;4,"W" &amp;  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>W1</v>
+        <v>Team 8</v>
       </c>
       <c r="E20" t="str">
         <f>IFERROR(
@@ -1269,13 +1257,13 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[BottomKey]],Table1[LoserTo],0))),
 IF(LEN(INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&gt;4,INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),"W" &amp; INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>Team 9</v>
+        <v>W2</v>
       </c>
       <c r="H20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I20" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="J20" t="str">
         <f>IFERROR(
@@ -1283,16 +1271,16 @@
 ISERROR(MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0)),
     "B" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[BottomKey],0)),
     "T" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0))),"")</f>
-        <v>T9</v>
+        <v>T10</v>
       </c>
       <c r="K20" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "B13", loser: "T9", topSource: "W1", bottomSource: "Team 9" },</v>
+        <v>{ winner: "T12", loser: "T10", topSource: "Team 8", bottomSource: "W2" },</v>
       </c>
     </row>
     <row r="21" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D21" t="str">
         <f>IFERROR(
@@ -1300,7 +1288,7 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[TopKey]],Table1[LoserTo],0))),
 IF(LEN( INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&lt;4,"W" &amp;  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>Team 10</v>
+        <v>L3</v>
       </c>
       <c r="E21" t="str">
         <f>IFERROR(
@@ -1308,13 +1296,16 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[BottomKey]],Table1[LoserTo],0))),
 IF(LEN(INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&gt;4,INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),"W" &amp; INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>W2</v>
-      </c>
-      <c r="H21" t="s">
-        <v>24</v>
+        <v>L2</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" t="s">
+        <v>19</v>
       </c>
       <c r="I21" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="J21" t="str">
         <f>IFERROR(
@@ -1322,16 +1313,16 @@
 ISERROR(MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0)),
     "B" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[BottomKey],0)),
     "T" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0))),"")</f>
-        <v>T12</v>
+        <v/>
       </c>
       <c r="K21" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "T14", loser: "T12", topSource: "Team 10", bottomSource: "W2" },</v>
+        <v>{ winner: "T9", loser: "", topSource: "L3", bottomSource: "L2" },</v>
       </c>
     </row>
     <row r="22" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C22">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D22" t="str">
         <f>IFERROR(
@@ -1339,7 +1330,7 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[TopKey]],Table1[LoserTo],0))),
 IF(LEN( INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&lt;4,"W" &amp;  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>W3</v>
+        <v>L1</v>
       </c>
       <c r="E22" t="str">
         <f>IFERROR(
@@ -1347,13 +1338,16 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[BottomKey]],Table1[LoserTo],0))),
 IF(LEN(INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&gt;4,INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),"W" &amp; INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>Team 11</v>
-      </c>
-      <c r="H22" t="s">
-        <v>25</v>
+        <v>L4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" t="s">
+        <v>20</v>
       </c>
       <c r="I22" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="J22" t="str">
         <f>IFERROR(
@@ -1361,16 +1355,16 @@
 ISERROR(MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0)),
     "B" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[BottomKey],0)),
     "T" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0))),"")</f>
-        <v>B10</v>
+        <v/>
       </c>
       <c r="K22" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "B14", loser: "B10", topSource: "W3", bottomSource: "Team 11" },</v>
+        <v>{ winner: "B10", loser: "", topSource: "L1", bottomSource: "L4" },</v>
       </c>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C23">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D23" t="str">
         <f>IFERROR(
@@ -1378,7 +1372,7 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[TopKey]],Table1[LoserTo],0))),
 IF(LEN( INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&lt;4,"W" &amp;  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>L4</v>
+        <v>W7</v>
       </c>
       <c r="E23" t="str">
         <f>IFERROR(
@@ -1386,16 +1380,13 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[BottomKey]],Table1[LoserTo],0))),
 IF(LEN(INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&gt;4,INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),"W" &amp; INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>L2</v>
-      </c>
-      <c r="F23" t="s">
-        <v>22</v>
+        <v>L5</v>
       </c>
       <c r="G23" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I23" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="J23" t="str">
         <f>IFERROR(
@@ -1407,12 +1398,12 @@
       </c>
       <c r="K23" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "T11", loser: "", topSource: "L4", bottomSource: "L2" },</v>
+        <v>{ winner: "B14", loser: "", topSource: "W7", bottomSource: "L5" },</v>
       </c>
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D24" t="str">
         <f>IFERROR(
@@ -1420,7 +1411,7 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[TopKey]],Table1[LoserTo],0))),
 IF(LEN( INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&lt;4,"W" &amp;  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>L5</v>
+        <v>L6</v>
       </c>
       <c r="E24" t="str">
         <f>IFERROR(
@@ -1428,16 +1419,13 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[BottomKey]],Table1[LoserTo],0))),
 IF(LEN(INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&gt;4,INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),"W" &amp; INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>L3</v>
+        <v>W8</v>
       </c>
       <c r="F24" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I24" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="J24" t="str">
         <f>IFERROR(
@@ -1449,12 +1437,12 @@
       </c>
       <c r="K24" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "B11", loser: "", topSource: "L5", bottomSource: "L3" },</v>
+        <v>{ winner: "T13", loser: "", topSource: "L6", bottomSource: "W8" },</v>
       </c>
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C25">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D25" t="str">
         <f>IFERROR(
@@ -1462,7 +1450,7 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[TopKey]],Table1[LoserTo],0))),
 IF(LEN( INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&lt;4,"W" &amp;  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>L1</v>
+        <v>W3</v>
       </c>
       <c r="E25" t="str">
         <f>IFERROR(
@@ -1470,16 +1458,13 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[BottomKey]],Table1[LoserTo],0))),
 IF(LEN(INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&gt;4,INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),"W" &amp; INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>L7</v>
-      </c>
-      <c r="F25" t="s">
-        <v>19</v>
-      </c>
-      <c r="G25" t="s">
-        <v>25</v>
+        <v>W5</v>
+      </c>
+      <c r="H25" t="s">
+        <v>26</v>
       </c>
       <c r="I25" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="J25" t="str">
         <f>IFERROR(
@@ -1487,16 +1472,16 @@
 ISERROR(MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0)),
     "B" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[BottomKey],0)),
     "T" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0))),"")</f>
-        <v/>
+        <v>B13</v>
       </c>
       <c r="K25" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "B12", loser: "", topSource: "L1", bottomSource: "L7" },</v>
+        <v>{ winner: "T15", loser: "B13", topSource: "W3", bottomSource: "W5" },</v>
       </c>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C26">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D26" t="str">
         <f>IFERROR(
@@ -1504,7 +1489,7 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[TopKey]],Table1[LoserTo],0))),
 IF(LEN( INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&lt;4,"W" &amp;  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>W8</v>
+        <v>W6</v>
       </c>
       <c r="E26" t="str">
         <f>IFERROR(
@@ -1512,10 +1497,13 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[BottomKey]],Table1[LoserTo],0))),
 IF(LEN(INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&gt;4,INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),"W" &amp; INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>W9</v>
+        <v>W4</v>
+      </c>
+      <c r="H26" t="s">
+        <v>23</v>
       </c>
       <c r="I26" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="J26" t="str">
         <f>IFERROR(
@@ -1523,16 +1511,16 @@
 ISERROR(MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0)),
     "B" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[BottomKey],0)),
     "T" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0))),"")</f>
-        <v/>
+        <v>T14</v>
       </c>
       <c r="K26" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "B16", loser: "", topSource: "W8", bottomSource: "W9" },</v>
+        <v>{ winner: "B15", loser: "T14", topSource: "W6", bottomSource: "W4" },</v>
       </c>
     </row>
     <row r="27" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C27">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D27" t="str">
         <f>IFERROR(
@@ -1540,7 +1528,7 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[TopKey]],Table1[LoserTo],0))),
 IF(LEN( INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&lt;4,"W" &amp;  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>L6</v>
+        <v>W10</v>
       </c>
       <c r="E27" t="str">
         <f>IFERROR(
@@ -1548,13 +1536,13 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[BottomKey]],Table1[LoserTo],0))),
 IF(LEN(INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&gt;4,INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),"W" &amp; INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>W10</v>
-      </c>
-      <c r="F27" t="s">
-        <v>24</v>
+        <v>L11</v>
+      </c>
+      <c r="G27" t="s">
+        <v>26</v>
       </c>
       <c r="I27" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="J27" t="str">
         <f>IFERROR(
@@ -1566,12 +1554,12 @@
       </c>
       <c r="K27" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "T15", loser: "", topSource: "L6", bottomSource: "W10" },</v>
+        <v>{ winner: "B16", loser: "", topSource: "W10", bottomSource: "L11" },</v>
       </c>
     </row>
     <row r="28" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C28">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D28" t="str">
         <f>IFERROR(
@@ -1579,7 +1567,7 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[TopKey]],Table1[LoserTo],0))),
 IF(LEN( INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&lt;4,"W" &amp;  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>W4</v>
+        <v>L12</v>
       </c>
       <c r="E28" t="str">
         <f>IFERROR(
@@ -1587,13 +1575,13 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[BottomKey]],Table1[LoserTo],0))),
 IF(LEN(INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&gt;4,INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),"W" &amp; INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>W5</v>
-      </c>
-      <c r="H28" t="s">
-        <v>26</v>
+        <v>W9</v>
+      </c>
+      <c r="F28" t="s">
+        <v>23</v>
       </c>
       <c r="I28" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="J28" t="str">
         <f>IFERROR(
@@ -1601,16 +1589,16 @@
 ISERROR(MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0)),
     "B" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[BottomKey],0)),
     "T" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0))),"")</f>
-        <v>B15</v>
+        <v/>
       </c>
       <c r="K28" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "T17", loser: "B15", topSource: "W4", bottomSource: "W5" },</v>
+        <v>{ winner: "T16", loser: "", topSource: "L12", bottomSource: "W9" },</v>
       </c>
     </row>
     <row r="29" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C29">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D29" t="str">
         <f>IFERROR(
@@ -1618,7 +1606,7 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[TopKey]],Table1[LoserTo],0))),
 IF(LEN( INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&lt;4,"W" &amp;  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>W6</v>
+        <v>W11</v>
       </c>
       <c r="E29" t="str">
         <f>IFERROR(
@@ -1626,13 +1614,13 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[BottomKey]],Table1[LoserTo],0))),
 IF(LEN(INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&gt;4,INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),"W" &amp; INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>W7</v>
+        <v>W12</v>
       </c>
       <c r="H29" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I29" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J29" t="str">
         <f>IFERROR(
@@ -1640,16 +1628,16 @@
 ISERROR(MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0)),
     "B" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[BottomKey],0)),
     "T" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0))),"")</f>
-        <v>T16</v>
+        <v>T17</v>
       </c>
       <c r="K29" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "B17", loser: "T16", topSource: "W6", bottomSource: "W7" },</v>
+        <v>{ winner: "T18", loser: "T17", topSource: "W11", bottomSource: "W12" },</v>
       </c>
     </row>
     <row r="30" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C30">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D30" t="str">
         <f>IFERROR(
@@ -1657,7 +1645,7 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[TopKey]],Table1[LoserTo],0))),
 IF(LEN( INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&lt;4,"W" &amp;  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>W12</v>
+        <v>W14</v>
       </c>
       <c r="E30" t="str">
         <f>IFERROR(
@@ -1665,13 +1653,10 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[BottomKey]],Table1[LoserTo],0))),
 IF(LEN(INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&gt;4,INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),"W" &amp; INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>L13</v>
-      </c>
-      <c r="G30" t="s">
-        <v>26</v>
+        <v>W13</v>
       </c>
       <c r="I30" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="J30" t="str">
         <f>IFERROR(
@@ -1683,12 +1668,12 @@
       </c>
       <c r="K30" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "B18", loser: "", topSource: "W12", bottomSource: "L13" },</v>
+        <v>{ winner: "B17", loser: "", topSource: "W14", bottomSource: "W13" },</v>
       </c>
     </row>
     <row r="31" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C31">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D31" t="str">
         <f>IFERROR(
@@ -1696,7 +1681,7 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[TopKey]],Table1[LoserTo],0))),
 IF(LEN( INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&lt;4,"W" &amp;  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>L14</v>
+        <v>L15</v>
       </c>
       <c r="E31" t="str">
         <f>IFERROR(
@@ -1704,13 +1689,13 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[BottomKey]],Table1[LoserTo],0))),
 IF(LEN(INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&gt;4,INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),"W" &amp; INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>W11</v>
+        <v>W16</v>
       </c>
       <c r="F31" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I31" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="J31" t="str">
         <f>IFERROR(
@@ -1722,12 +1707,12 @@
       </c>
       <c r="K31" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "T18", loser: "", topSource: "L14", bottomSource: "W11" },</v>
+        <v>{ winner: "B18", loser: "", topSource: "L15", bottomSource: "W16" },</v>
       </c>
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C32">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D32" t="str">
         <f>IFERROR(
@@ -1735,7 +1720,7 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[TopKey]],Table1[LoserTo],0))),
 IF(LEN( INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&lt;4,"W" &amp;  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>W13</v>
+        <v>W15</v>
       </c>
       <c r="E32" t="str">
         <f>IFERROR(
@@ -1743,13 +1728,10 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[BottomKey]],Table1[LoserTo],0))),
 IF(LEN(INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&gt;4,INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),"W" &amp; INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>W14</v>
-      </c>
-      <c r="H32" t="s">
-        <v>28</v>
+        <v>W17</v>
       </c>
       <c r="I32" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="J32" t="str">
         <f>IFERROR(
@@ -1757,16 +1739,16 @@
 ISERROR(MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0)),
     "B" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[BottomKey],0)),
     "T" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0))),"")</f>
-        <v>T19</v>
+        <v/>
       </c>
       <c r="K32" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "T20", loser: "T19", topSource: "W13", bottomSource: "W14" },</v>
+        <v>{ winner: "T19", loser: "", topSource: "W15", bottomSource: "W17" },</v>
       </c>
     </row>
     <row r="33" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C33">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D33" t="str">
         <f>IFERROR(
@@ -1774,7 +1756,7 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[TopKey]],Table1[LoserTo],0))),
 IF(LEN( INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&lt;4,"W" &amp;  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>W16</v>
+        <v>W18</v>
       </c>
       <c r="E33" t="str">
         <f>IFERROR(
@@ -1782,10 +1764,16 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[BottomKey]],Table1[LoserTo],0))),
 IF(LEN(INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&gt;4,INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),"W" &amp; INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>W15</v>
+        <v>L19</v>
+      </c>
+      <c r="G33" t="s">
+        <v>27</v>
+      </c>
+      <c r="H33" t="s">
+        <v>27</v>
       </c>
       <c r="I33" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="J33" t="str">
         <f>IFERROR(
@@ -1793,16 +1781,16 @@
 ISERROR(MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0)),
     "B" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[BottomKey],0)),
     "T" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0))),"")</f>
-        <v/>
+        <v>B19</v>
       </c>
       <c r="K33" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "B19", loser: "", topSource: "W16", bottomSource: "W15" },</v>
+        <v>{ winner: "T20", loser: "B19", topSource: "W18", bottomSource: "L19" },</v>
       </c>
     </row>
     <row r="34" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C34">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D34" t="str">
         <f>IFERROR(
@@ -1810,7 +1798,7 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[TopKey]],Table1[LoserTo],0))),
 IF(LEN( INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&lt;4,"W" &amp;  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>L17</v>
+        <v>W19</v>
       </c>
       <c r="E34" t="str">
         <f>IFERROR(
@@ -1818,13 +1806,7 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[BottomKey]],Table1[LoserTo],0))),
 IF(LEN(INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&gt;4,INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),"W" &amp; INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>W18</v>
-      </c>
-      <c r="F34" t="s">
-        <v>28</v>
-      </c>
-      <c r="I34" t="s">
-        <v>48</v>
+        <v/>
       </c>
       <c r="J34" t="str">
         <f>IFERROR(
@@ -1836,12 +1818,12 @@
       </c>
       <c r="K34" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "B20", loser: "", topSource: "L17", bottomSource: "W18" },</v>
+        <v>{ winner: "", loser: "", topSource: "W19", bottomSource: "" },</v>
       </c>
     </row>
     <row r="35" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C35">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D35" t="str">
         <f>IFERROR(
@@ -1849,7 +1831,7 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[TopKey]],Table1[LoserTo],0))),
 IF(LEN( INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&lt;4,"W" &amp;  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>W17</v>
+        <v/>
       </c>
       <c r="E35" t="str">
         <f>IFERROR(
@@ -1857,13 +1839,7 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[BottomKey]],Table1[LoserTo],0))),
 IF(LEN(INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&gt;4,INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),"W" &amp; INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>W19</v>
-      </c>
-      <c r="H35" t="s">
-        <v>29</v>
-      </c>
-      <c r="I35" t="s">
-        <v>49</v>
+        <v/>
       </c>
       <c r="J35" t="str">
         <f>IFERROR(
@@ -1871,16 +1847,16 @@
 ISERROR(MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0)),
     "B" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[BottomKey],0)),
     "T" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0))),"")</f>
-        <v>B21</v>
+        <v/>
       </c>
       <c r="K35" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "T21", loser: "B21", topSource: "W17", bottomSource: "W19" },</v>
+        <v>{ winner: "", loser: "", topSource: "", bottomSource: "" },</v>
       </c>
     </row>
     <row r="36" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C36">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D36" t="str">
         <f>IFERROR(
@@ -1888,7 +1864,7 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[TopKey]],Table1[LoserTo],0))),
 IF(LEN( INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&lt;4,"W" &amp;  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>W20</v>
+        <v/>
       </c>
       <c r="E36" t="str">
         <f>IFERROR(
@@ -1896,13 +1872,7 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[BottomKey]],Table1[LoserTo],0))),
 IF(LEN(INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&gt;4,INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),"W" &amp; INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>L20</v>
-      </c>
-      <c r="G36" t="s">
-        <v>29</v>
-      </c>
-      <c r="I36" t="s">
-        <v>62</v>
+        <v/>
       </c>
       <c r="J36" t="str">
         <f>IFERROR(
@@ -1914,12 +1884,12 @@
       </c>
       <c r="K36" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "T22", loser: "", topSource: "W20", bottomSource: "L20" },</v>
+        <v>{ winner: "", loser: "", topSource: "", bottomSource: "" },</v>
       </c>
     </row>
     <row r="37" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C37">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D37" t="str">
         <f>IFERROR(
@@ -1927,7 +1897,7 @@
 _xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[TopKey]],Table1[LoserTo],0))),
 IF(LEN( INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&lt;4,"W" &amp;  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
 ),"")</f>
-        <v>W21</v>
+        <v/>
       </c>
       <c r="E37" t="str">
         <f>IFERROR(
@@ -1947,12 +1917,12 @@
       </c>
       <c r="K37" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "", loser: "", topSource: "W21", bottomSource: "" },</v>
+        <v>{ winner: "", loser: "", topSource: "", bottomSource: "" },</v>
       </c>
     </row>
     <row r="38" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C38">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D38" t="str">
         <f>IFERROR(
@@ -1985,7 +1955,7 @@
     </row>
     <row r="39" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C39">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D39" t="str">
         <f>IFERROR(
@@ -2018,7 +1988,7 @@
     </row>
     <row r="40" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C40">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D40" t="str">
         <f>IFERROR(
@@ -2051,7 +2021,7 @@
     </row>
     <row r="41" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C41">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D41" t="str">
         <f>IFERROR(
@@ -2084,7 +2054,7 @@
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C42">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D42" t="str">
         <f>IFERROR(
@@ -2117,7 +2087,7 @@
     </row>
     <row r="43" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C43">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D43" t="str">
         <f>IFERROR(
@@ -2150,7 +2120,7 @@
     </row>
     <row r="44" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C44">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D44" t="str">
         <f>IFERROR(
@@ -2183,7 +2153,7 @@
     </row>
     <row r="45" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C45">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D45" t="str">
         <f>IFERROR(
@@ -2216,7 +2186,7 @@
     </row>
     <row r="46" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C46">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D46" t="str">
         <f>IFERROR(
@@ -2249,7 +2219,7 @@
     </row>
     <row r="47" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C47">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D47" t="str">
         <f>IFERROR(
@@ -2282,7 +2252,7 @@
     </row>
     <row r="48" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C48">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D48" t="str">
         <f>IFERROR(
@@ -2315,7 +2285,7 @@
     </row>
     <row r="49" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C49">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D49" t="str">
         <f>IFERROR(
@@ -2348,7 +2318,7 @@
     </row>
     <row r="50" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C50">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D50" t="str">
         <f>IFERROR(
@@ -2381,7 +2351,7 @@
     </row>
     <row r="51" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C51">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D51" t="str">
         <f>IFERROR(
@@ -2408,39 +2378,6 @@
         <v/>
       </c>
       <c r="K51" t="str">
-        <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
-        <v>{ winner: "", loser: "", topSource: "", bottomSource: "" },</v>
-      </c>
-    </row>
-    <row r="52" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C52">
-        <v>37</v>
-      </c>
-      <c r="D52" t="str">
-        <f>IFERROR(
-IF(Table1[[#This Row],[TopKey]]&lt;&gt;"",
-_xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[TopKey]],Table1[LoserTo],0))),
-IF(LEN( INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&lt;4,"W" &amp;  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),  INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("T",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
-),"")</f>
-        <v/>
-      </c>
-      <c r="E52" t="str">
-        <f>IFERROR(
-IF(Table1[[#This Row],[BottomKey]]&lt;&gt;"",
-_xlfn.CONCAT("L",INDEX(Table1[Column1],MATCH(Table1[[#This Row],[BottomKey]],Table1[LoserTo],0))),
-IF(LEN(INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))&gt;4,INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)),"W" &amp; INDEX(Table1[Column1], MATCH(_xlfn.CONCAT("B",Table1[[#This Row],[Column1]]),Table1[WinnerTo],0)))
-),"")</f>
-        <v/>
-      </c>
-      <c r="J52" t="str">
-        <f>IFERROR(
-IF(
-ISERROR(MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0)),
-    "B" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[BottomKey],0)),
-    "T" &amp; INDEX(Table1[Column1], MATCH(Table1[[#This Row],[LoserTo]],Table1[TopKey],0))),"")</f>
-        <v/>
-      </c>
-      <c r="K52" t="str">
         <f>"{ winner: """ &amp; Table1[[#This Row],[WinnerTo]] &amp; """, loser: """ &amp; Table1[[#This Row],[LosertTo2]] &amp; """, topSource: """ &amp; Table1[[#This Row],[Top]] &amp; """, bottomSource: """ &amp; Table1[[#This Row],[Bottom]] &amp; """ },"</f>
         <v>{ winner: "", loser: "", topSource: "", bottomSource: "" },</v>
       </c>

</xml_diff>